<commit_message>
Log updates for Burn-Up List, and time estimations updated.
</commit_message>
<xml_diff>
--- a/logs/SmithIan_TimeEstimations.xlsx
+++ b/logs/SmithIan_TimeEstimations.xlsx
@@ -846,8 +846,8 @@
   </sheetPr>
   <dimension ref="B1:J28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1040,10 +1040,12 @@
       <c r="C14" s="18">
         <v>3</v>
       </c>
-      <c r="D14" s="21"/>
+      <c r="D14" s="21">
+        <v>3</v>
+      </c>
       <c r="E14" s="19">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1053,10 +1055,12 @@
       <c r="C15" s="18">
         <v>2</v>
       </c>
-      <c r="D15" s="21"/>
+      <c r="D15" s="21">
+        <v>1</v>
+      </c>
       <c r="E15" s="19">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1066,10 +1070,12 @@
       <c r="C16" s="18">
         <v>4</v>
       </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="21">
+        <v>1</v>
+      </c>
       <c r="E16" s="19">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1079,10 +1085,12 @@
       <c r="C17" s="18">
         <v>3</v>
       </c>
-      <c r="D17" s="21"/>
+      <c r="D17" s="21">
+        <v>2</v>
+      </c>
       <c r="E17" s="19">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1092,10 +1100,12 @@
       <c r="C18" s="18">
         <v>3.5</v>
       </c>
-      <c r="D18" s="21"/>
+      <c r="D18" s="21">
+        <v>2</v>
+      </c>
       <c r="E18" s="19">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1113,44 +1123,52 @@
       <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="18">
+        <v>3</v>
+      </c>
       <c r="D20" s="21"/>
       <c r="E20" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="18"/>
+      <c r="C21" s="18">
+        <v>4</v>
+      </c>
       <c r="D21" s="21"/>
       <c r="E21" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="18"/>
+      <c r="C22" s="18">
+        <v>2</v>
+      </c>
       <c r="D22" s="21"/>
       <c r="E22" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="18"/>
+      <c r="C23" s="18">
+        <v>2</v>
+      </c>
       <c r="D23" s="21"/>
       <c r="E23" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>